<commit_message>
almost done with exp4
</commit_message>
<xml_diff>
--- a/experiment4/experiment4.xlsx
+++ b/experiment4/experiment4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kubilayagi/Documents/UCLA/physics4al/experiment4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7264D903-05AD-5649-A5BB-CA9D81D6AAE6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A829F8-2415-E049-A72F-C464ED29EE56}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="1080" windowWidth="30600" windowHeight="17880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1880" yWindow="1080" windowWidth="30600" windowHeight="17880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
@@ -14909,8 +14909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1205"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -50169,8 +50169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>